<commit_message>
added some buttons to test the regression to the GUI
</commit_message>
<xml_diff>
--- a/robotTracking/bin/Debug/bandwidthResultsGraph.xlsx
+++ b/robotTracking/bin/Debug/bandwidthResultsGraph.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15300" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="bandwidthResults" sheetId="1" r:id="rId1"/>
@@ -572,6 +572,35 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Mean</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> error (mm) vs bandwidth</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -630,313 +659,313 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>1E-3</c:v>
+                  <c:v>1E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2E-3</c:v>
+                  <c:v>2.0000000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>2.9999999999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.9999999999999995E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.9999999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.0000000000000004E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.9999999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.9999989999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.1999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4E-3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.5E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.6999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.8E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.8999990000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.9999990000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.099999E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.2000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.3E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.3999999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.5000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.5999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.7000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.8E-3</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2.8999999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="29">
                   <c:v>3.0000000000000001E-3</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.0000009999999996E-3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7.0000009999999996E-3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.0000000000000002E-3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9.0000010000000005E-3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.01</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.0999999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.2E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.2999999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.4E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.4999999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1.6E-2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.7000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>1.7999999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>1.9E-2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2.1000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2.1999999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2.3E-2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>2.4E-2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>2.5000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>2.5999999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>2.7E-2</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>2.8000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>2.9000000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>0.03</c:v>
-                </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.1E-2</c:v>
+                  <c:v>3.0999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.2000000000000001E-2</c:v>
+                  <c:v>3.2000000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.3000000000000002E-2</c:v>
+                  <c:v>3.3E-3</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.4000000000000002E-2</c:v>
+                  <c:v>3.3999999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.5000000000000003E-2</c:v>
+                  <c:v>3.5000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.5999990000000003E-2</c:v>
+                  <c:v>3.5999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.6999990000000003E-2</c:v>
+                  <c:v>3.7000000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>3.7999989999999997E-2</c:v>
+                  <c:v>3.8000009999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3.8999989999999998E-2</c:v>
+                  <c:v>3.9000010000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>3.9999989999999999E-2</c:v>
+                  <c:v>4.0000010000000004E-3</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4.099999E-2</c:v>
+                  <c:v>4.1000000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4.1999979999999999E-2</c:v>
+                  <c:v>4.1999999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4.299998E-2</c:v>
+                  <c:v>4.3E-3</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4.3999980000000001E-2</c:v>
+                  <c:v>4.4000000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4.4999980000000002E-2</c:v>
+                  <c:v>4.4999999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4.5999980000000003E-2</c:v>
+                  <c:v>4.5999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4.6999979999999997E-2</c:v>
+                  <c:v>4.6999989999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4.7999970000000003E-2</c:v>
+                  <c:v>4.7999990000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4.8999969999999997E-2</c:v>
+                  <c:v>4.8999990000000004E-3</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4.9999969999999998E-2</c:v>
+                  <c:v>4.9999989999999998E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>bandwidthResults!$B$1:$B$50</c:f>
+              <c:f>bandwidthResults!$C$1:$C$50</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>34.781010000000002</c:v>
+                  <c:v>14.84567</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29.671320000000001</c:v>
+                  <c:v>14.8431</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.121079999999999</c:v>
+                  <c:v>14.38796</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.83663</c:v>
+                  <c:v>12.391310000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.204910000000002</c:v>
+                  <c:v>10.219610000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.716349999999998</c:v>
+                  <c:v>8.7742339999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23.33689</c:v>
+                  <c:v>8.0746789999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23.066770000000002</c:v>
+                  <c:v>7.8683199999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22.893329999999999</c:v>
+                  <c:v>7.872331</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>22.796410000000002</c:v>
+                  <c:v>8.0241600000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22.756170000000001</c:v>
+                  <c:v>8.3223120000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22.756730000000001</c:v>
+                  <c:v>8.7753069999999997</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>22.78668</c:v>
+                  <c:v>9.3828499999999995</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>22.838259999999998</c:v>
+                  <c:v>10.131609999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>22.906189999999999</c:v>
+                  <c:v>11.0014</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>22.986920000000001</c:v>
+                  <c:v>11.967560000000001</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23.078060000000001</c:v>
+                  <c:v>13.00365</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>23.178070000000002</c:v>
+                  <c:v>14.085179999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>23.286000000000001</c:v>
+                  <c:v>15.190570000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>23.401199999999999</c:v>
+                  <c:v>16.301500000000001</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>23.523209999999999</c:v>
+                  <c:v>17.402930000000001</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>23.651579999999999</c:v>
+                  <c:v>18.482959999999999</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>23.785889999999998</c:v>
+                  <c:v>19.532440000000001</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23.925609999999999</c:v>
+                  <c:v>20.544689999999999</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24.070209999999999</c:v>
+                  <c:v>21.515079999999998</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>24.219059999999999</c:v>
+                  <c:v>22.440740000000002</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>24.37154</c:v>
+                  <c:v>23.320209999999999</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>24.52703</c:v>
+                  <c:v>24.15316</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>24.68487</c:v>
+                  <c:v>24.940049999999999</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>24.844460000000002</c:v>
+                  <c:v>25.68206</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>25.005220000000001</c:v>
+                  <c:v>26.38072</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>25.166609999999999</c:v>
+                  <c:v>27.03792</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>25.328140000000001</c:v>
+                  <c:v>27.6557</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>25.489329999999999</c:v>
+                  <c:v>28.23621</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>25.649819999999998</c:v>
+                  <c:v>28.781610000000001</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>25.80921</c:v>
+                  <c:v>29.294029999999999</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>25.967199999999998</c:v>
+                  <c:v>29.775559999999999</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>26.1235</c:v>
+                  <c:v>30.228209999999997</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>26.27786</c:v>
+                  <c:v>30.6539</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>26.43009</c:v>
+                  <c:v>31.05443</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>26.580010000000001</c:v>
+                  <c:v>31.431470000000004</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>26.727450000000001</c:v>
+                  <c:v>31.786679999999997</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>26.872309999999999</c:v>
+                  <c:v>32.121470000000002</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>27.014469999999999</c:v>
+                  <c:v>32.437280000000001</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>27.153860000000002</c:v>
+                  <c:v>32.735370000000003</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>27.290420000000001</c:v>
+                  <c:v>33.016959999999997</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>27.42409</c:v>
+                  <c:v>33.283140000000003</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>27.554849999999998</c:v>
+                  <c:v>33.534929999999996</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>27.682690000000001</c:v>
+                  <c:v>33.773329999999994</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>27.807569999999998</c:v>
+                  <c:v>33.999160000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -951,11 +980,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="496395096"/>
-        <c:axId val="496394704"/>
+        <c:axId val="539872344"/>
+        <c:axId val="539871952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="496395096"/>
+        <c:axId val="539872344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1012,12 +1041,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496394704"/>
+        <c:crossAx val="539871952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="496394704"/>
+        <c:axId val="539871952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1074,7 +1103,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="496395096"/>
+        <c:crossAx val="539872344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1683,16 +1712,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>501162</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>184638</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>196361</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>70338</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1977,412 +2006,619 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B50"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
       <c r="B1">
-        <v>34.781010000000002</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.484567E-2</v>
+      </c>
+      <c r="C1">
+        <f>B1*1000</f>
+        <v>14.84567</v>
+      </c>
+      <c r="E1">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="F1">
+        <f>MIN(C1:C50)</f>
+        <v>7.8683199999999998</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2E-3</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="B2">
-        <v>29.671320000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1.48431E-2</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:C50" si="0">B2*1000</f>
+        <v>14.8431</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="B3">
+        <v>1.438796E-2</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>14.38796</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="B4">
+        <v>1.2391310000000001E-2</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>12.391310000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="B5">
+        <v>1.021961E-2</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>10.219610000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="B6">
+        <v>8.7742340000000005E-3</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>8.7742339999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="B7">
+        <v>8.0746789999999995E-3</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>8.0746789999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="B8">
+        <v>7.8683199999999998E-3</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>7.8683199999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="B9">
+        <v>7.8723309999999998E-3</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>7.872331</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9.9999989999999999E-4</v>
+      </c>
+      <c r="B10">
+        <v>8.0241600000000007E-3</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>8.0241600000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="B11">
+        <v>8.3223120000000001E-3</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>8.3223120000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="B12">
+        <v>8.7753069999999996E-3</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>8.7753069999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="B13">
+        <v>9.3828499999999999E-3</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>9.3828499999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1.4E-3</v>
+      </c>
+      <c r="B14">
+        <v>1.0131609999999999E-2</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>10.131609999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>1.5E-3</v>
+      </c>
+      <c r="B15">
+        <v>1.10014E-2</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>11.0014</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="B16">
+        <v>1.196756E-2</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>11.967560000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1.6999999999999999E-3</v>
+      </c>
+      <c r="B17">
+        <v>1.300365E-2</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>13.00365</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1.8E-3</v>
+      </c>
+      <c r="B18">
+        <v>1.4085179999999999E-2</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>14.085179999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1.8999990000000001E-3</v>
+      </c>
+      <c r="B19">
+        <v>1.519057E-2</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>15.190570000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1.9999990000000001E-3</v>
+      </c>
+      <c r="B20">
+        <v>1.63015E-2</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>16.301500000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2.099999E-3</v>
+      </c>
+      <c r="B21">
+        <v>1.740293E-2</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>17.402930000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="B22">
+        <v>1.848296E-2</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>18.482959999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2.3E-3</v>
+      </c>
+      <c r="B23">
+        <v>1.9532440000000002E-2</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>19.532440000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="B24">
+        <v>2.0544690000000001E-2</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>20.544689999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="B25">
+        <v>2.1515079999999999E-2</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>21.515079999999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2.5999999999999999E-3</v>
+      </c>
+      <c r="B26">
+        <v>2.2440740000000001E-2</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>22.440740000000002</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2.7000000000000001E-3</v>
+      </c>
+      <c r="B27">
+        <v>2.3320210000000001E-2</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>23.320209999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2.8E-3</v>
+      </c>
+      <c r="B28">
+        <v>2.415316E-2</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>24.15316</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2.8999999999999998E-3</v>
+      </c>
+      <c r="B29">
+        <v>2.4940049999999998E-2</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>24.940049999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="B3">
-        <v>26.121079999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="B4">
-        <v>24.83663</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="B5">
-        <v>24.204910000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>6.0000009999999996E-3</v>
-      </c>
-      <c r="B6">
-        <v>23.716349999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>7.0000009999999996E-3</v>
-      </c>
-      <c r="B7">
-        <v>23.33689</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="B8">
-        <v>23.066770000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>9.0000010000000005E-3</v>
-      </c>
-      <c r="B9">
-        <v>22.893329999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>0.01</v>
-      </c>
-      <c r="B10">
-        <v>22.796410000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="B11">
-        <v>22.756170000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1.2E-2</v>
-      </c>
-      <c r="B12">
-        <v>22.756730000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="B13">
-        <v>22.78668</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1.4E-2</v>
-      </c>
-      <c r="B14">
-        <v>22.838259999999998</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="B15">
-        <v>22.906189999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1.6E-2</v>
-      </c>
-      <c r="B16">
-        <v>22.986920000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="B17">
-        <v>23.078060000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="B18">
-        <v>23.178070000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>1.9E-2</v>
-      </c>
-      <c r="B19">
-        <v>23.286000000000001</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>0.02</v>
-      </c>
-      <c r="B20">
-        <v>23.401199999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="B21">
-        <v>23.523209999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="B22">
-        <v>23.651579999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>2.3E-2</v>
-      </c>
-      <c r="B23">
-        <v>23.785889999999998</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>2.4E-2</v>
-      </c>
-      <c r="B24">
-        <v>23.925609999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="B25">
-        <v>24.070209999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="B26">
-        <v>24.219059999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>2.7E-2</v>
-      </c>
-      <c r="B27">
-        <v>24.37154</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>2.8000000000000001E-2</v>
-      </c>
-      <c r="B28">
-        <v>24.52703</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="B29">
-        <v>24.68487</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>0.03</v>
-      </c>
       <c r="B30">
-        <v>24.844460000000002</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2.568206E-2</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>25.68206</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>3.1E-2</v>
+        <v>3.0999999999999999E-3</v>
       </c>
       <c r="B31">
-        <v>25.005220000000001</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2.638072E-2</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>26.38072</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>3.2000000000000001E-2</v>
+        <v>3.2000000000000002E-3</v>
       </c>
       <c r="B32">
-        <v>25.166609999999999</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2.703792E-2</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>27.03792</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>3.3000000000000002E-2</v>
+        <v>3.3E-3</v>
       </c>
       <c r="B33">
-        <v>25.328140000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2.7655699999999998E-2</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>27.6557</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>3.4000000000000002E-2</v>
+        <v>3.3999999999999998E-3</v>
       </c>
       <c r="B34">
-        <v>25.489329999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2.8236210000000001E-2</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>28.23621</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>3.5000000000000003E-2</v>
+        <v>3.5000000000000001E-3</v>
       </c>
       <c r="B35">
-        <v>25.649819999999998</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2.8781609999999999E-2</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>28.781610000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>3.5999990000000003E-2</v>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="B36">
-        <v>25.80921</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2.9294029999999999E-2</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>29.294029999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>3.6999990000000003E-2</v>
+        <v>3.7000000000000002E-3</v>
       </c>
       <c r="B37">
-        <v>25.967199999999998</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2.977556E-2</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>29.775559999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>3.7999989999999997E-2</v>
+        <v>3.8000009999999999E-3</v>
       </c>
       <c r="B38">
-        <v>26.1235</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3.0228209999999998E-2</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>30.228209999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>3.8999989999999998E-2</v>
+        <v>3.9000010000000002E-3</v>
       </c>
       <c r="B39">
-        <v>26.27786</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3.0653900000000001E-2</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>30.6539</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>3.9999989999999999E-2</v>
+        <v>4.0000010000000004E-3</v>
       </c>
       <c r="B40">
-        <v>26.43009</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3.1054430000000001E-2</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>31.05443</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>4.099999E-2</v>
+        <v>4.1000000000000003E-3</v>
       </c>
       <c r="B41">
-        <v>26.580010000000001</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3.1431470000000003E-2</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>31.431470000000004</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>4.1999979999999999E-2</v>
+        <v>4.1999999999999997E-3</v>
       </c>
       <c r="B42">
-        <v>26.727450000000001</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3.1786679999999998E-2</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>31.786679999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>4.299998E-2</v>
+        <v>4.3E-3</v>
       </c>
       <c r="B43">
-        <v>26.872309999999999</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3.2121469999999999E-2</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>32.121470000000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>4.3999980000000001E-2</v>
+        <v>4.4000000000000003E-3</v>
       </c>
       <c r="B44">
-        <v>27.014469999999999</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3.2437279999999999E-2</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>32.437280000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>4.4999980000000002E-2</v>
+        <v>4.4999999999999997E-3</v>
       </c>
       <c r="B45">
-        <v>27.153860000000002</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3.273537E-2</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>32.735370000000003</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>4.5999980000000003E-2</v>
+        <v>4.5999999999999999E-3</v>
       </c>
       <c r="B46">
-        <v>27.290420000000001</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3.3016959999999998E-2</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>33.016959999999997</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>4.6999979999999997E-2</v>
+        <v>4.6999989999999998E-3</v>
       </c>
       <c r="B47">
-        <v>27.42409</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3.3283140000000003E-2</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>33.283140000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>4.7999970000000003E-2</v>
+        <v>4.7999990000000001E-3</v>
       </c>
       <c r="B48">
-        <v>27.554849999999998</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3.3534929999999998E-2</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>33.534929999999996</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>4.8999969999999997E-2</v>
+        <v>4.8999990000000004E-3</v>
       </c>
       <c r="B49">
-        <v>27.682690000000001</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3.3773329999999997E-2</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>33.773329999999994</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>4.9999969999999998E-2</v>
+        <v>4.9999989999999998E-3</v>
       </c>
       <c r="B50">
-        <v>27.807569999999998</v>
+        <v>3.399916E-2</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>33.999160000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more to thesis regarding feature scaling
</commit_message>
<xml_diff>
--- a/robotTracking/bin/Debug/bandwidthResultsGraph.xlsx
+++ b/robotTracking/bin/Debug/bandwidthResultsGraph.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="bandwidthResults" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -578,12 +578,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -591,12 +588,20 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB"/>
+              <a:rPr lang="en-GB" sz="1800" b="1" u="none">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t>Mean</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> error (mm) vs bandwidth</a:t>
+              <a:rPr lang="en-GB" sz="1800" b="1" u="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> error  vs Bandwidth for regression function</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -615,12 +620,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -641,16 +643,26 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
@@ -980,11 +992,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="539872344"/>
-        <c:axId val="539871952"/>
+        <c:axId val="556386736"/>
+        <c:axId val="556387128"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="539872344"/>
+        <c:axId val="556386736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -995,8 +1007,7 @@
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                  <a:alpha val="40000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -1004,6 +1015,175 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1800" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Bandwidth (dimensionless)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="556387128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="556387128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1800" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Mean Positional Error (mm)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1041,69 +1221,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539871952"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="539871952"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="539872344"/>
+        <c:crossAx val="556386736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1125,10 +1243,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="tx1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -1712,16 +1827,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>185459</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>180694</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>89647</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2009,7 +2124,7 @@
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>